<commit_message>
Updated the sprintTask Sheet
</commit_message>
<xml_diff>
--- a/SprintTaskSheet.xlsx
+++ b/SprintTaskSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t xml:space="preserve">Week #1 (10 hrs / week)</t>
   </si>
@@ -213,6 +213,9 @@
   </si>
   <si>
     <t xml:space="preserve">For Admin, Add rental locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add and update database using queries for individual vehicles and rental locations.</t>
   </si>
   <si>
     <t xml:space="preserve">For Admin, Add vehicles and vehicle Types</t>
@@ -484,7 +487,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -654,10 +657,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -753,7 +752,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -801,6 +800,223 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
+              <a:srgbClr val="dc3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="19080">
+              <a:solidFill>
+                <a:srgbClr val="dc3912"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$E$3:$AG$3</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2/25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2/26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2/27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2/28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2/29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3/2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3/3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3/4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3/5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3/6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3/7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3/8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3/9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3/10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3/11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3/12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3/13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3/14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3/15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3/16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3/17</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3/18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3/19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3/20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3/21</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3/22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3/23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$E$5:$AG$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
               <a:srgbClr val="3366cc">
                 <a:alpha val="30000"/>
               </a:srgbClr>
@@ -1013,228 +1229,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="dc3912">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="19080">
-              <a:solidFill>
-                <a:srgbClr val="dc3912"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sprint!$E$3:$AG$3</c:f>
-              <c:strCache>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2/25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2/26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2/27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2/29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3/2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3/3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3/4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3/5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3/6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3/7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3/8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3/9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3/10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3/11</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3/12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3/13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3/14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3/15</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3/16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3/17</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3/18</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3/19</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3/20</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3/21</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3/22</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3/23</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sprint!$E$5:$AG$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="84894366"/>
-        <c:axId val="23700033"/>
+        <c:axId val="62467467"/>
+        <c:axId val="31728363"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="84894366"/>
+        <c:axId val="62467467"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,14 +1299,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23700033"/>
+        <c:crossAx val="31728363"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23700033"/>
+        <c:axId val="31728363"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1380,7 +1379,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84894366"/>
+        <c:crossAx val="62467467"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1441,9 +1440,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>992160</xdr:colOff>
+      <xdr:colOff>991800</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>123120</xdr:rowOff>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1452,7 +1451,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="390600" y="609120"/>
-        <a:ext cx="9762480" cy="4914360"/>
+        <a:ext cx="9762120" cy="4914000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1472,8 +1471,8 @@
   </sheetPr>
   <dimension ref="A1:AG34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2441,7 +2440,9 @@
       <c r="B22" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="41"/>
+      <c r="C22" s="41" t="s">
+        <v>44</v>
+      </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41"/>
       <c r="F22" s="41"/>
@@ -2461,7 +2462,7 @@
       <c r="T22" s="41"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="44" t="s">
+      <c r="B23" s="43" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="41"/>
@@ -2484,7 +2485,7 @@
       <c r="T23" s="41"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="41"/>
@@ -2507,7 +2508,7 @@
       <c r="T24" s="41"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>62</v>
       </c>
       <c r="C25" s="41"/>
@@ -2529,9 +2530,12 @@
       <c r="S25" s="41"/>
       <c r="T25" s="41"/>
     </row>
-    <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="44" t="s">
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="43" t="s">
         <v>63</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
@@ -2552,9 +2556,9 @@
       <c r="S26" s="41"/>
       <c r="T26" s="41"/>
     </row>
-    <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="44" t="s">
-        <v>64</v>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="43" t="s">
+        <v>65</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -2576,7 +2580,7 @@
       <c r="T27" s="41"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="44"/>
+      <c r="B28" s="43"/>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
@@ -2597,8 +2601,8 @@
       <c r="T28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="45" t="s">
-        <v>65</v>
+      <c r="A29" s="44" t="s">
+        <v>66</v>
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
@@ -2620,11 +2624,11 @@
       <c r="T29" s="41"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="46" t="s">
-        <v>66</v>
+      <c r="A30" s="45" t="s">
+        <v>67</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
@@ -2646,11 +2650,11 @@
       <c r="T30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="46" t="s">
+      <c r="A31" s="45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="41" t="s">
         <v>68</v>
-      </c>
-      <c r="B31" s="41" t="s">
-        <v>67</v>
       </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
@@ -2672,11 +2676,11 @@
       <c r="T31" s="41"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="46" t="s">
-        <v>69</v>
+      <c r="A32" s="45" t="s">
+        <v>70</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
@@ -2698,10 +2702,10 @@
       <c r="T32" s="41"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="B33" s="47" t="n">
+      <c r="A33" s="46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B33" s="46" t="n">
         <f aca="false">97</f>
         <v>97</v>
       </c>
@@ -3728,32 +3732,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="48"/>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
path changed to /user
</commit_message>
<xml_diff>
--- a/SprintTaskSheet.xlsx
+++ b/SprintTaskSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
   <si>
     <t xml:space="preserve">Week #1 (10 hrs / week)</t>
   </si>
@@ -219,6 +219,18 @@
   </si>
   <si>
     <t xml:space="preserve">For Admin, Add vehicles and vehicle Types</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User Authentication n authorization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Architecture Diagram and documentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AWS with load balancer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Login for user and admin</t>
   </si>
   <si>
     <t xml:space="preserve">Team:</t>
@@ -752,7 +764,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -800,6 +812,223 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
+              <a:srgbClr val="3366cc">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="19080">
+              <a:solidFill>
+                <a:srgbClr val="3366cc"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$E$3:$AG$3</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2/25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2/26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2/27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2/28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2/29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3/2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3/3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3/4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3/5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3/6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3/7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3/8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3/9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3/10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3/11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3/12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3/13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3/14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3/15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3/16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3/17</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3/18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3/19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3/20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3/21</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3/22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3/23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$E$4:$AG$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
               <a:srgbClr val="dc3912">
                 <a:alpha val="30000"/>
               </a:srgbClr>
@@ -1012,228 +1241,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="3366cc">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="19080">
-              <a:solidFill>
-                <a:srgbClr val="3366cc"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sprint!$E$3:$AG$3</c:f>
-              <c:strCache>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2/25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2/26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2/27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2/29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3/2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3/3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3/4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3/5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3/6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3/7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3/8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3/9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3/10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3/11</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3/12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3/13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3/14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3/15</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3/16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3/17</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3/18</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3/19</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3/20</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3/21</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3/22</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3/23</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sprint!$E$4:$AG$4</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>97</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>95</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>93</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>89</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>85</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>83</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>79</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>75</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>73</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="62467467"/>
-        <c:axId val="31728363"/>
+        <c:axId val="27045951"/>
+        <c:axId val="73152596"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="62467467"/>
+        <c:axId val="27045951"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,14 +1311,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31728363"/>
+        <c:crossAx val="73152596"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="31728363"/>
+        <c:axId val="73152596"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1379,7 +1391,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="62467467"/>
+        <c:crossAx val="27045951"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1440,9 +1452,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>991800</xdr:colOff>
+      <xdr:colOff>991440</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>122760</xdr:rowOff>
+      <xdr:rowOff>122400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1451,7 +1463,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="390600" y="609120"/>
-        <a:ext cx="9762120" cy="4914000"/>
+        <a:ext cx="9761760" cy="4913640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1469,13 +1481,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG34"/>
+  <dimension ref="A1:AG38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="49.42"/>
@@ -2465,7 +2477,9 @@
       <c r="B23" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="41"/>
+      <c r="C23" s="41" t="s">
+        <v>42</v>
+      </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
       <c r="F23" s="41"/>
@@ -2488,7 +2502,9 @@
       <c r="B24" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="41"/>
+      <c r="C24" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
       <c r="F24" s="41"/>
@@ -2511,7 +2527,9 @@
       <c r="B25" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="41"/>
+      <c r="C25" s="41" t="s">
+        <v>42</v>
+      </c>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
       <c r="F25" s="41"/>
@@ -2537,7 +2555,9 @@
       <c r="B26" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="41"/>
+      <c r="C26" s="41" t="s">
+        <v>42</v>
+      </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
       <c r="F26" s="41"/>
@@ -2580,8 +2600,12 @@
       <c r="T27" s="41"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="43"/>
-      <c r="C28" s="41"/>
+      <c r="B28" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="D28" s="41"/>
       <c r="E28" s="41"/>
       <c r="F28" s="41"/>
@@ -2600,11 +2624,13 @@
       <c r="S28" s="41"/>
       <c r="T28" s="41"/>
     </row>
-    <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="44" t="s">
-        <v>66</v>
-      </c>
-      <c r="C29" s="41"/>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="41" t="s">
+        <v>42</v>
+      </c>
       <c r="D29" s="41"/>
       <c r="E29" s="41"/>
       <c r="F29" s="41"/>
@@ -2623,14 +2649,13 @@
       <c r="S29" s="41"/>
       <c r="T29" s="41"/>
     </row>
-    <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="41" t="s">
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="43" t="s">
         <v>68</v>
       </c>
-      <c r="C30" s="41"/>
+      <c r="C30" s="41" t="s">
+        <v>44</v>
+      </c>
       <c r="D30" s="41"/>
       <c r="E30" s="41"/>
       <c r="F30" s="41"/>
@@ -2649,14 +2674,13 @@
       <c r="S30" s="41"/>
       <c r="T30" s="41"/>
     </row>
-    <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="45" t="s">
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="43" t="s">
         <v>69</v>
       </c>
-      <c r="B31" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="C31" s="41"/>
+      <c r="C31" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="D31" s="41"/>
       <c r="E31" s="41"/>
       <c r="F31" s="41"/>
@@ -2675,13 +2699,8 @@
       <c r="S31" s="41"/>
       <c r="T31" s="41"/>
     </row>
-    <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B32" s="41" t="s">
-        <v>68</v>
-      </c>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="43"/>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
@@ -2701,14 +2720,8 @@
       <c r="S32" s="41"/>
       <c r="T32" s="41"/>
     </row>
-    <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="46" t="n">
-        <f aca="false">97</f>
-        <v>97</v>
-      </c>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="43"/>
       <c r="C33" s="41"/>
       <c r="D33" s="41"/>
       <c r="E33" s="41"/>
@@ -2728,972 +2741,44 @@
       <c r="S33" s="41"/>
       <c r="T33" s="41"/>
     </row>
-    <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="166" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="167" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="168" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="169" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="170" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="171" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="172" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="173" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="174" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="175" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="176" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="177" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="178" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="179" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="180" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="181" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="182" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="183" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="184" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="185" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="186" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="187" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="188" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="189" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="190" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="191" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="192" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="193" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="194" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="195" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="196" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="197" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="198" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="199" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="200" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="201" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="202" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="203" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="204" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="205" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="206" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="207" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="208" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="209" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="210" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="211" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="212" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="213" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="214" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="215" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="216" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="217" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="218" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="219" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="220" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="221" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="222" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="223" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="224" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="225" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="226" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="227" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="228" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="229" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="230" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="231" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="232" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="233" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="234" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="235" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="236" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="237" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="238" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="239" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="240" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="241" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="242" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="243" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="244" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="245" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="246" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="247" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="248" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="249" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="250" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="251" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="252" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="253" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="254" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="255" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="256" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="257" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="258" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="259" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="260" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="261" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="262" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="263" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="264" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="265" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="266" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="267" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="268" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="269" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="270" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="271" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="272" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="273" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="274" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="275" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="276" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="277" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="278" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="279" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="280" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="281" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="282" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="283" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="284" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="285" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="286" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="287" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="288" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="289" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="290" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="291" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="292" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="293" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="294" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="295" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="296" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="297" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="298" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="299" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="300" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="301" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="302" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="303" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="304" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="305" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="306" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="307" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="308" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="309" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="310" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="311" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="312" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="313" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="314" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="315" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="316" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="317" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="318" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="319" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="320" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="321" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="322" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="323" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="324" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="325" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="326" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="327" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="328" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="329" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="330" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="331" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="332" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="333" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="334" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="335" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="336" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="337" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="338" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="339" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="340" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="341" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="342" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="343" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="344" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="345" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="346" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="347" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="348" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="349" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="350" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="351" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="352" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="353" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="354" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="355" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="356" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="357" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="358" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="359" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="360" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="361" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="362" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="363" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="364" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="365" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="366" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="367" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="368" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="369" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="370" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="371" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="372" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="373" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="374" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="375" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="376" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="377" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="378" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="379" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="380" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="381" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="382" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="383" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="384" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="385" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="386" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="387" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="388" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="389" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="390" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="391" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="392" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="393" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="394" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="395" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="396" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="397" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="398" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="399" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="400" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="401" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="402" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="403" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="404" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="405" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="406" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="407" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="408" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="409" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="410" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="411" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="412" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="413" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="414" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="415" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="416" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="417" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="418" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="419" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="420" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="421" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="422" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="423" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="424" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="425" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="426" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="427" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="428" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="429" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="430" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="431" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="432" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="433" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="434" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="435" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="436" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="437" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="438" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="439" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="440" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="441" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="442" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="443" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="444" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="445" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="446" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="447" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="448" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="449" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="450" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="451" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="452" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="453" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="454" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="455" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="456" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="457" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="458" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="459" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="460" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="461" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="462" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="463" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="464" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="465" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="466" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="467" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="468" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="469" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="470" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="471" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="472" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="473" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="474" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="475" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="476" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="477" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="478" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="479" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="480" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="481" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="482" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="483" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="484" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="485" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="486" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="487" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="488" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="489" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="490" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="491" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="492" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="493" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="494" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="495" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="496" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="497" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="498" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="499" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="500" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="501" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="502" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="503" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="504" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="505" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="506" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="507" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="508" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="509" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="510" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="511" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="512" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="513" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="514" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="515" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="516" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="517" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="518" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="519" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="520" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="521" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="522" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="523" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="524" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="525" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="526" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="527" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="528" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="529" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="530" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="531" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="532" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="533" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="534" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="535" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="536" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="537" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="538" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="539" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="540" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="541" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="542" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="543" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="544" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="545" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="546" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="547" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="548" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="549" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="550" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="551" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="552" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="553" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="554" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="555" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="556" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="557" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="558" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="559" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="560" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="561" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="562" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="563" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="564" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="565" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="566" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="567" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="568" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="569" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="570" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="571" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="572" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="573" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="574" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="575" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="576" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="577" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="578" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="579" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="580" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="581" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="582" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="583" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="584" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="585" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="586" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="587" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="588" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="589" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="590" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="591" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="592" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="593" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="594" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="595" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="596" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="597" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="598" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="599" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="600" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="601" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="602" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="603" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="604" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="605" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="606" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="607" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="608" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="609" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="610" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="611" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="612" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="613" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="614" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="615" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="616" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="617" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="618" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="619" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="620" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="621" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="622" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="623" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="624" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="625" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="626" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="627" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="628" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="629" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="630" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="631" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="632" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="633" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="634" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="635" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="636" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="637" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="638" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="639" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="640" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="641" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="642" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="643" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="644" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="645" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="646" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="647" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="648" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="649" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="650" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="651" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="652" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="653" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="654" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="655" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="656" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="657" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="658" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="659" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="660" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="661" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="662" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="663" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="664" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="665" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="666" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="667" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="668" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="669" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="670" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="671" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="672" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="673" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="674" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="675" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="676" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="677" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="678" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="679" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="680" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="681" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="682" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="683" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="684" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="685" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="686" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="687" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="688" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="689" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="690" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="691" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="692" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="693" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="694" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="695" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="696" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="697" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="698" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="699" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="700" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="701" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="702" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="703" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="704" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="705" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="706" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="707" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="708" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="709" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="710" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="711" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="712" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="713" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="714" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="715" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="716" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="717" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="718" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="719" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="720" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="721" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="722" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="723" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="724" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="725" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="726" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="727" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="728" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="729" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="730" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="731" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="732" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="733" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="734" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="735" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="736" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="737" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="738" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="739" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="740" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="741" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="742" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="743" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="744" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="745" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="746" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="747" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="748" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="749" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="750" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="751" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="752" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="753" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="754" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="755" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="756" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="757" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="758" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="759" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="760" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="761" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="762" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="763" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="764" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="765" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="766" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="767" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="768" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="769" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="770" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="771" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="772" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="773" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="774" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="775" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="776" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="777" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="778" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="779" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="780" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="781" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="782" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="783" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="784" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="785" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="786" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="787" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="788" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="789" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="790" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="791" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="792" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="793" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="794" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="795" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="796" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="797" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="798" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="799" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="800" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="801" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="802" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="803" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="804" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="805" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="806" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="807" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="808" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="809" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="810" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="811" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="812" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="813" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="814" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="815" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="816" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="817" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="818" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="819" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="820" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="821" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="822" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="823" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="824" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="825" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="826" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="827" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="828" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="829" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="830" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="831" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="832" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="833" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="834" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="835" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="836" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="837" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="838" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="839" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="840" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="841" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="842" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="843" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="844" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="845" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="846" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="847" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="848" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="849" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="850" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="851" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="852" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="853" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="854" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="855" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="856" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="857" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="858" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="859" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="860" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="861" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="862" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="863" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="864" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="865" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="866" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="867" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="868" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="869" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="870" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="871" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="872" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="873" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="874" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="875" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="876" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="877" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="878" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="879" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="880" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="881" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="882" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="883" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="884" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="885" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="886" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="887" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="888" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="889" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="890" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="891" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="892" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="893" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="894" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="895" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="896" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="897" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="898" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="899" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="900" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="901" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="902" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="903" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="904" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="905" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="906" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="907" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="908" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="909" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="910" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="911" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="912" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="913" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="914" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="915" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="916" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="917" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="918" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="919" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="920" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="921" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="922" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="923" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="924" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="925" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="926" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="927" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="928" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="929" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="930" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="931" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="932" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="933" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="934" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="935" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="936" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="937" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="938" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="939" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="940" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="941" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="942" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="943" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="944" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="945" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="946" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="947" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="948" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="949" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="950" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="951" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="952" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="953" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="954" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="955" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="956" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="957" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="958" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="959" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="960" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="961" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="962" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="963" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="964" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="965" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="966" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="967" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="968" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="969" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="970" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="971" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="972" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="973" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="974" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="975" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="976" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="977" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="978" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="979" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="980" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="981" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="982" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="983" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="984" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="985" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="986" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="987" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="988" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="989" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="990" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="991" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="992" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="997" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="998" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="999" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="B35" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="B36" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="B37" s="41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="46" t="n">
+        <f aca="false">97</f>
+        <v>97</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E1:K1"/>

</xml_diff>

<commit_message>
Updated Weekly Scrum Task Board
</commit_message>
<xml_diff>
--- a/SprintTaskSheet.xlsx
+++ b/SprintTaskSheet.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="84">
   <si>
     <t xml:space="preserve">Week #1 (10 hrs / week)</t>
   </si>
@@ -188,6 +188,33 @@
     <t xml:space="preserve">Front End Design Discussion</t>
   </si>
   <si>
+    <t xml:space="preserve">Design User Registration functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete User Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search and Browse rental location and vehicles functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">My reservation tab with option to Cancel and Return</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Backend Implementation for Search and Browse functionality.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> UI design for Vehicle reservation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete the Vehicle reservation functionality</t>
+  </si>
+  <si>
+    <t xml:space="preserve">React and Node application deployment on AWS EC2.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attaching Load balancer wih auto scaling groups to EC2. </t>
+  </si>
+  <si>
     <t xml:space="preserve">User Registration</t>
   </si>
   <si>
@@ -195,9 +222,6 @@
   </si>
   <si>
     <t xml:space="preserve">Search and Browse rental location and vehicles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">My reservation tab with option to Cancel and Return</t>
   </si>
   <si>
     <t xml:space="preserve">Vehicle reservation and validation</t>
@@ -259,7 +283,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M\/D"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -304,6 +328,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -499,7 +529,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -672,12 +702,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -685,6 +739,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -812,6 +870,223 @@
           <c:order val="0"/>
           <c:spPr>
             <a:solidFill>
+              <a:srgbClr val="dc3912">
+                <a:alpha val="30000"/>
+              </a:srgbClr>
+            </a:solidFill>
+            <a:ln w="19080">
+              <a:solidFill>
+                <a:srgbClr val="dc3912"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sprint!$E$3:$AG$3</c:f>
+              <c:strCache>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2/25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2/26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2/27</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2/28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2/29</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3/1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3/2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3/3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3/4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3/5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3/6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3/7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3/8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3/9</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3/10</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3/11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3/12</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3/13</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3/14</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3/15</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3/16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3/17</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3/18</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3/19</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3/20</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3/21</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3/22</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3/23</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sprint!$E$5:$AG$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v/>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:solidFill>
               <a:srgbClr val="3366cc">
                 <a:alpha val="30000"/>
               </a:srgbClr>
@@ -1024,228 +1299,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="dc3912">
-                <a:alpha val="30000"/>
-              </a:srgbClr>
-            </a:solidFill>
-            <a:ln w="19080">
-              <a:solidFill>
-                <a:srgbClr val="dc3912"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sprint!$E$3:$AG$3</c:f>
-              <c:strCache>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2/25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2/26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2/27</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2/28</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2/29</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3/1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>3/2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>3/3</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3/4</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3/5</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3/6</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3/7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3/8</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3/9</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3/10</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3/11</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3/12</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3/13</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3/14</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3/15</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3/16</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3/17</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3/18</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3/19</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3/20</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3/21</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3/22</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3/23</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sprint!$E$5:$AG$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="29"/>
-                <c:pt idx="0">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:axId val="27045951"/>
-        <c:axId val="73152596"/>
+        <c:axId val="19431210"/>
+        <c:axId val="81393651"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="27045951"/>
+        <c:axId val="19431210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1311,14 +1369,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73152596"/>
+        <c:crossAx val="81393651"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73152596"/>
+        <c:axId val="81393651"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1391,7 +1449,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27045951"/>
+        <c:crossAx val="19431210"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1452,9 +1510,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>991440</xdr:colOff>
+      <xdr:colOff>991080</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>122400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1463,7 +1521,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="390600" y="609120"/>
-        <a:ext cx="9761760" cy="4913640"/>
+        <a:ext cx="9761400" cy="4913280"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1481,10 +1539,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG38"/>
+  <dimension ref="A1:AG51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1982,7 +2040,9 @@
       <c r="AF7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="31"/>
+      <c r="A8" s="31" t="n">
+        <v>1</v>
+      </c>
       <c r="B8" s="19" t="s">
         <v>43</v>
       </c>
@@ -2062,7 +2122,9 @@
       <c r="AF9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="32"/>
+      <c r="A10" s="32" t="n">
+        <v>2</v>
+      </c>
       <c r="B10" s="33" t="s">
         <v>46</v>
       </c>
@@ -2142,7 +2204,9 @@
       <c r="AF11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="38"/>
+      <c r="A12" s="38" t="n">
+        <v>3</v>
+      </c>
       <c r="B12" s="39" t="s">
         <v>49</v>
       </c>
@@ -2266,7 +2330,9 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="35"/>
+      <c r="A15" s="35" t="n">
+        <v>4</v>
+      </c>
       <c r="B15" s="42" t="s">
         <v>52</v>
       </c>
@@ -2348,15 +2414,16 @@
       <c r="S17" s="41"/>
       <c r="T17" s="41"/>
     </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="39" t="s">
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="38" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="44"/>
       <c r="F18" s="41"/>
       <c r="G18" s="41"/>
       <c r="H18" s="41"/>
@@ -2373,15 +2440,14 @@
       <c r="S18" s="41"/>
       <c r="T18" s="41"/>
     </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="39" t="s">
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="38"/>
+      <c r="B19" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="44"/>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
       <c r="H19" s="41"/>
@@ -2398,15 +2464,14 @@
       <c r="S19" s="41"/>
       <c r="T19" s="41"/>
     </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="39" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="38"/>
+      <c r="B20" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
@@ -2423,15 +2488,14 @@
       <c r="S20" s="41"/>
       <c r="T20" s="41"/>
     </row>
-    <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="39" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="38"/>
+      <c r="B21" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="C21" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="44"/>
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
@@ -2448,15 +2512,16 @@
       <c r="S21" s="41"/>
       <c r="T21" s="41"/>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="43" t="s">
+    <row r="22" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="35" t="n">
+        <v>6</v>
+      </c>
+      <c r="B22" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="C22" s="37"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="44"/>
       <c r="F22" s="41"/>
       <c r="G22" s="41"/>
       <c r="H22" s="41"/>
@@ -2473,15 +2538,14 @@
       <c r="S22" s="41"/>
       <c r="T22" s="41"/>
     </row>
-    <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="43" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="35"/>
+      <c r="B23" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="C23" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="44"/>
       <c r="F23" s="41"/>
       <c r="G23" s="41"/>
       <c r="H23" s="41"/>
@@ -2498,15 +2562,16 @@
       <c r="S23" s="41"/>
       <c r="T23" s="41"/>
     </row>
-    <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="38" t="n">
+        <v>7</v>
+      </c>
       <c r="B24" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="44"/>
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
@@ -2523,15 +2588,14 @@
       <c r="S24" s="41"/>
       <c r="T24" s="41"/>
     </row>
-    <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="43" t="s">
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="35"/>
+      <c r="B25" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="C25" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="44"/>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
@@ -2549,17 +2613,13 @@
       <c r="T25" s="41"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="35"/>
+      <c r="B26" s="47" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="44"/>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
@@ -2577,12 +2637,11 @@
       <c r="T26" s="41"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="49"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="44"/>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
@@ -2599,15 +2658,12 @@
       <c r="S27" s="41"/>
       <c r="T27" s="41"/>
     </row>
-    <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="43" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="48"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="44"/>
+      <c r="E28" s="44"/>
       <c r="F28" s="41"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
@@ -2625,14 +2681,11 @@
       <c r="T28" s="41"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="43" t="s">
-        <v>67</v>
-      </c>
-      <c r="C29" s="41" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="A29" s="48"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
       <c r="F29" s="41"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
@@ -2650,14 +2703,11 @@
       <c r="T29" s="41"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="43" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="41" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="A30" s="48"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
       <c r="F30" s="41"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
@@ -2675,8 +2725,8 @@
       <c r="T30" s="41"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="43" t="s">
-        <v>69</v>
+      <c r="B31" s="49" t="s">
+        <v>64</v>
       </c>
       <c r="C31" s="41" t="s">
         <v>47</v>
@@ -2700,8 +2750,12 @@
       <c r="T31" s="41"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="43"/>
-      <c r="C32" s="41"/>
+      <c r="B32" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="41" t="s">
+        <v>47</v>
+      </c>
       <c r="D32" s="41"/>
       <c r="E32" s="41"/>
       <c r="F32" s="41"/>
@@ -2721,8 +2775,12 @@
       <c r="T32" s="41"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="43"/>
-      <c r="C33" s="41"/>
+      <c r="B33" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="41" t="s">
+        <v>44</v>
+      </c>
       <c r="D33" s="41"/>
       <c r="E33" s="41"/>
       <c r="F33" s="41"/>
@@ -2742,39 +2800,149 @@
       <c r="T33" s="41"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="44" t="s">
+      <c r="B34" s="49" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D34" s="41"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="50" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="41"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" s="41"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" s="41"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="50" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="45" t="s">
+      <c r="C38" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D38" s="41"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B39" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="45" t="s">
+      <c r="C39" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D39" s="41"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="50" t="s">
         <v>73</v>
       </c>
-      <c r="B36" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="45" t="s">
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="B37" s="41" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="46" t="s">
+      <c r="C41" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="41"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="46" t="n">
+      <c r="C42" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="41"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B43" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="D43" s="41"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B44" s="50" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="41"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="41"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="50"/>
+      <c r="C46" s="41"/>
+      <c r="D46" s="41"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="51" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="B49" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="52" t="s">
+        <v>82</v>
+      </c>
+      <c r="B50" s="41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="53" t="s">
+        <v>83</v>
+      </c>
+      <c r="B51" s="53" t="n">
         <f aca="false">97</f>
         <v>97</v>
       </c>
@@ -2817,32 +2985,32 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47"/>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="N1" s="47"/>
-      <c r="O1" s="47"/>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47"/>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47"/>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="A1" s="54"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>